<commit_message>
add generating new id from last id of Book1
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -2,20 +2,20 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookPr backupFile="false" date1904="false" showObjects="all"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="985" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" r:id="rId2" sheetId="1" state="visible"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="0" name="ID" vbProcedure="false">Sheet1!$A$1</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="LASTUPDATEDATE" vbProcedure="false">Sheet1!$C$1</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="TITLE" vbProcedure="false">Sheet1!$B$1</definedName>
   </definedNames>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr iterate="false" iterateCount="100" iterateDelta="0.001" refMode="A1"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -111,14 +111,14 @@
     </fill>
   </fills>
   <borders count="2">
-    <border diagonalUp="false" diagonalDown="false">
+    <border diagonalDown="false" diagonalUp="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border diagonalDown="false" diagonalUp="false">
       <left style="hair"/>
       <right style="hair"/>
       <top style="hair"/>
@@ -127,59 +127,59 @@
     </border>
   </borders>
   <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="4" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
+    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
+    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
+    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
+    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
+    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -251,16 +251,16 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A3" activeCellId="0" pane="topLeft" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="12.8295454545455"/>
+    <col min="1" max="1025" hidden="false" style="0" width="8.72159090909091" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -271,7 +271,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
@@ -282,10 +282,15 @@
         <v>42728</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="true" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,標準"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,標準"&amp;12ページ &amp;P</oddFooter>

</xml_diff>

<commit_message>
get cell names from target sheet.
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -2,20 +2,22 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" date1904="false" showObjects="all"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="985" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" r:id="rId2" sheetId="1" state="visible"/>
+    <sheet name="Sheet2" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="ID" vbProcedure="false">Sheet1!$A$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="LASTUPDATEDATE" vbProcedure="false">Sheet1!$C$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="TITLE" vbProcedure="false">Sheet1!$B$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="ID" vbProcedure="false">Sheet2!$B$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="ID" vbProcedure="false">Sheet1!$A$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="LASTUPDATEDATE" vbProcedure="false">Sheet1!$C$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="TITLE" vbProcedure="false">Sheet1!$B$1</definedName>
   </definedNames>
-  <calcPr iterate="false" iterateCount="100" iterateDelta="0.001" refMode="A1"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -111,14 +113,14 @@
     </fill>
   </fills>
   <borders count="2">
-    <border diagonalDown="false" diagonalUp="false">
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
+    <border diagonalUp="false" diagonalDown="false">
       <left style="hair"/>
       <right style="hair"/>
       <top style="hair"/>
@@ -127,59 +129,59 @@
     </border>
   </borders>
   <cellStyleXfs count="20">
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
-    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
-    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
-    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
-    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -249,18 +251,44 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="B1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A3" activeCellId="0" pane="topLeft" sqref="A3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col min="1" max="1025" hidden="false" style="0" width="8.72159090909091" collapsed="true"/>
-  </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="0" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,標準"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,標準"&amp;12ページ &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -271,7 +299,7 @@
         <v>2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
@@ -282,15 +310,10 @@
         <v>42728</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2.0</v>
-      </c>
-    </row>
   </sheetData>
-  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="true" usePrinterDefaults="false" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,標準"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,標準"&amp;12ページ &amp;P</oddFooter>

</xml_diff>

<commit_message>
add inserting input text to sheet2.xlsx
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -153,8 +153,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -258,9 +262,12 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.72159090909091"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -283,30 +290,33 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.72159090909091"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="4" t="n">
+      <c r="C2" s="5" t="n">
         <v>42728</v>
       </c>
     </row>

</xml_diff>